<commit_message>
add support for time.Time data type on row struct
</commit_message>
<xml_diff>
--- a/sample/sample.xlsx
+++ b/sample/sample.xlsx
@@ -4,13 +4,13 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12180"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28680" windowHeight="11880"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$G$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$H$7</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="13">
   <si>
     <t>ID</t>
   </si>
@@ -52,6 +52,15 @@
   </si>
   <si>
     <t>xxx@gmail.com</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Date 2</t>
+  </si>
+  <si>
+    <t>2022-09-20</t>
   </si>
 </sst>
 </file>
@@ -110,13 +119,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -398,11 +409,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -413,9 +422,11 @@
     <col min="5" max="5" width="23.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.140625" customWidth="1"/>
+    <col min="9" max="9" width="20.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -437,8 +448,14 @@
       <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="H1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -460,8 +477,14 @@
       <c r="G2" s="5">
         <v>44</v>
       </c>
+      <c r="H2" s="6">
+        <v>44824.56459490741</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>2</v>
       </c>
@@ -483,8 +506,14 @@
       <c r="G3" s="5">
         <v>44</v>
       </c>
+      <c r="H3" s="6">
+        <v>44824.56459490741</v>
+      </c>
+      <c r="I3" s="7" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>3</v>
       </c>
@@ -506,8 +535,14 @@
       <c r="G4" s="5">
         <v>44</v>
       </c>
+      <c r="H4" s="6">
+        <v>44824.56459490741</v>
+      </c>
+      <c r="I4" s="7" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="5" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>4</v>
       </c>
@@ -529,8 +564,14 @@
       <c r="G5" s="5">
         <v>44</v>
       </c>
+      <c r="H5" s="6">
+        <v>44824.56459490741</v>
+      </c>
+      <c r="I5" s="7" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="6" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>5</v>
       </c>
@@ -552,8 +593,14 @@
       <c r="G6" s="5">
         <v>44</v>
       </c>
+      <c r="H6" s="6">
+        <v>44824.56459490741</v>
+      </c>
+      <c r="I6" s="7" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="7" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>6</v>
       </c>
@@ -575,9 +622,15 @@
       <c r="G7" s="5">
         <v>44</v>
       </c>
+      <c r="H7" s="6">
+        <v>44824.56459490741</v>
+      </c>
+      <c r="I7" s="7" t="s">
+        <v>12</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G1"/>
+  <autoFilter ref="A1:H7"/>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1"/>
     <hyperlink ref="D2" r:id="rId2"/>

</xml_diff>